<commit_message>
Changed the logic for the component's part
</commit_message>
<xml_diff>
--- a/src/main/resources/cobigen-licenses-include.xlsx
+++ b/src/main/resources/cobigen-licenses-include.xlsx
@@ -2,27 +2,30 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiazgon\Desktop\Contract_License\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" tabRatio="896"/>
   </bookViews>
   <sheets>
     <sheet name="SELECTION" sheetId="1" r:id="rId1"/>
     <sheet name="cobigen-core" sheetId="5" r:id="rId2"/>
     <sheet name="cobigen-eclipse" sheetId="6" r:id="rId3"/>
     <sheet name="cobigen-maven" sheetId="7" r:id="rId4"/>
+    <sheet name="cobigen-javaplugin" sheetId="9" r:id="rId5"/>
+    <sheet name="cobigen-propertyplugin" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="av_core">t_av_core[cobigen-core]</definedName>
     <definedName name="av_eclipse">t_av_eclipse[cobigen-eclipse]</definedName>
+    <definedName name="av_java">t_av_java[cobigen-javaplugin]</definedName>
     <definedName name="av_maven">t_av_maven[cobigen-maven]</definedName>
+    <definedName name="av_property">t_av_property[cobigen-propertyplugin]</definedName>
     <definedName name="languages">t_desc[Language]</definedName>
-    <definedName name="test">t_desc[Language]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="68">
   <si>
     <t>cobigen-core</t>
   </si>
@@ -165,20 +168,86 @@
     <t>Embedded Components</t>
   </si>
   <si>
-    <t>Selected</t>
-  </si>
-  <si>
     <t>Main Applications</t>
   </si>
   <si>
-    <t>v.1.4.0</t>
+    <t>CobiGen Java Plug-in</t>
+  </si>
+  <si>
+    <t>QDox</t>
+  </si>
+  <si>
+    <t>2.0-M3</t>
+  </si>
+  <si>
+    <t>Mature Modular Meta-Framework (mmm-util-pojo)</t>
+  </si>
+  <si>
+    <t>cobigen-javaplugin</t>
+  </si>
+  <si>
+    <t>CobiGen Property Plug-in</t>
+  </si>
+  <si>
+    <t>v1.1.1</t>
+  </si>
+  <si>
+    <t>cobigen-propertyplugin</t>
+  </si>
+  <si>
+    <t>v2.1.0</t>
+  </si>
+  <si>
+    <t>Logback-classic</t>
+  </si>
+  <si>
+    <t>LGLP 2.1, EPL v1.0</t>
+  </si>
+  <si>
+    <t>Apache Ant</t>
+  </si>
+  <si>
+    <t>Apache Licence 2.0</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>1.9.6</t>
+  </si>
+  <si>
+    <t>v3.0.0</t>
+  </si>
+  <si>
+    <t>Maven-plugin-api</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Maven-core</t>
+  </si>
+  <si>
+    <t>Maven-compat</t>
+  </si>
+  <si>
+    <t>Maven-plugin-annotations</t>
+  </si>
+  <si>
+    <t>v1.6.0</t>
+  </si>
+  <si>
+    <t>v1.2.0</t>
+  </si>
+  <si>
+    <t>DE:Noch ein Kommentar.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +289,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -296,7 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -347,15 +422,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="59">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -459,7 +562,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -563,17 +674,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -677,6 +784,226 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -724,126 +1051,182 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="t_desc" displayName="t_desc" ref="F2:G4" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="t_desc" displayName="t_desc" ref="F2:G4" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <tableColumns count="2">
-    <tableColumn id="1" name="Language" dataDxfId="31"/>
-    <tableColumn id="2" name="Description" dataDxfId="30"/>
+    <tableColumn id="1" name="Language" dataDxfId="56"/>
+    <tableColumn id="2" name="Description" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="t_dep_core_4101316" displayName="t_dep_core_4101316" ref="E20:G29" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4">
-  <autoFilter ref="E20:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="t_av_maven" displayName="t_av_maven" ref="B4:B7" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-maven" dataDxfId="22"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="t_dep_java_150" displayName="t_dep_java_150" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="3"/>
-    <tableColumn id="2" name="Version" dataDxfId="2"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="1"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="21"/>
+    <tableColumn id="2" name="Version" dataDxfId="20"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="t_av_maven" displayName="t_av_maven" ref="B4:B6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B4:B6"/>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="t_dep_core_41013163" displayName="t_dep_core_41013163" ref="E17:G21" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="E17:G21"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="16"/>
+    <tableColumn id="2" name="Version" dataDxfId="15"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="t_av_java" displayName="t_av_java" ref="B4:B7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-maven"/>
+    <tableColumn id="1" name="cobigen-javaplugin" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="t_dep_java_1505" displayName="t_dep_java_1505" ref="E8:G9" totalsRowShown="0">
+  <autoFilter ref="E8:G9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="10"/>
+    <tableColumn id="2" name="Version" dataDxfId="9"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="t_dep_core_410131636" displayName="t_dep_core_410131636" ref="E15:G16" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6">
+  <autoFilter ref="E15:G16"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="5"/>
+    <tableColumn id="2" name="Version" dataDxfId="4"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="t_av_property" displayName="t_av_property" ref="B4:B7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-propertyplugin" dataDxfId="0">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="t_dep_core_400" displayName="t_dep_core_400" ref="E8:G16" totalsRowShown="0">
-  <autoFilter ref="E8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="t_dep_core_400" displayName="t_dep_core_400" ref="E8:G17" totalsRowShown="0">
+  <autoFilter ref="E8:G17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="29"/>
-    <tableColumn id="2" name="Version" dataDxfId="28"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="27"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="54"/>
+    <tableColumn id="2" name="Version" dataDxfId="53"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="t_dep_core_410" displayName="t_dep_core_410" ref="E20:G29" totalsRowShown="0" headerRowBorderDxfId="26" tableBorderDxfId="25">
-  <autoFilter ref="E20:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="t_dep_core_410" displayName="t_dep_core_410" ref="E20:G28" totalsRowShown="0" headerRowBorderDxfId="51" tableBorderDxfId="50">
+  <autoFilter ref="E20:G28"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="24"/>
-    <tableColumn id="2" name="Version" dataDxfId="23"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="22"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="49"/>
+    <tableColumn id="2" name="Version" dataDxfId="48"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="t_av_core" displayName="t_av_core" ref="B4:B6" totalsRowShown="0" headerRowDxfId="21">
-  <autoFilter ref="B4:B6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="t_av_core" displayName="t_av_core" ref="B4:B7" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+  <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-core"/>
+    <tableColumn id="1" name="cobigen-core" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="t_dep_core_40018" displayName="t_dep_core_40018" ref="K8:M16" totalsRowShown="0">
-  <autoFilter ref="K8:M16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="t_dep_core_40012" displayName="t_dep_core_40012" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="20">
-      <calculatedColumnFormula>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K9:$K$9)),1,1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="2" name="Version" dataDxfId="19"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="18"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="43"/>
+    <tableColumn id="2" name="Version" dataDxfId="42"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="t_dep_core_40012" displayName="t_dep_core_40012" ref="E8:G16" totalsRowShown="0">
-  <autoFilter ref="E8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="t_dep_core_41013" displayName="t_dep_core_41013" ref="E17:G26" totalsRowShown="0" headerRowBorderDxfId="40" tableBorderDxfId="39">
+  <autoFilter ref="E17:G26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="17"/>
-    <tableColumn id="2" name="Version" dataDxfId="16"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="15"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="38"/>
+    <tableColumn id="2" name="Version" dataDxfId="37"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="t_dep_core_41013" displayName="t_dep_core_41013" ref="E20:G29" totalsRowShown="0" headerRowBorderDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="E20:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="t_av_eclipse" displayName="t_av_eclipse" ref="B4:B7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-eclipse" dataDxfId="33"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="t_dep_core_4001215" displayName="t_dep_core_4001215" ref="E8:G14" totalsRowShown="0">
+  <autoFilter ref="E8:G14"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="12"/>
-    <tableColumn id="2" name="Version" dataDxfId="11"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="10"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="32"/>
+    <tableColumn id="2" name="Version" dataDxfId="31"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="t_av_eclipse" displayName="t_av_eclipse" ref="B4:B6" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="B4:B6"/>
-  <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-eclipse"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="t_dep_core_4001215" displayName="t_dep_core_4001215" ref="E8:G16" totalsRowShown="0">
-  <autoFilter ref="E8:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="t_dep_core_4101316" displayName="t_dep_core_4101316" ref="E20:G26" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28">
+  <autoFilter ref="E20:G26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="8"/>
-    <tableColumn id="2" name="Version" dataDxfId="7"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="6"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="27"/>
+    <tableColumn id="2" name="Version" dataDxfId="26"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1115,14 +1498,14 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="17.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="18" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="18"/>
     <col min="6" max="6" width="9.7109375" style="18" customWidth="1"/>
     <col min="7" max="7" width="53.85546875" style="18" bestFit="1" customWidth="1"/>
@@ -1218,7 +1601,7 @@
     <row r="10" spans="1:9" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="21"/>
       <c r="B10" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
@@ -1236,7 +1619,7 @@
         <v>cobigen-eclipse</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21" t="str">
@@ -1255,7 +1638,7 @@
         <v>cobigen-maven</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="21" t="str">
@@ -1336,15 +1719,18 @@
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
       <c r="B18" s="21"/>
-      <c r="C18" s="21" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="C18" s="21" t="str">
+        <f>t_av_java[[#Headers],[cobigen-javaplugin]]</f>
+        <v>cobigen-javaplugin</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="21" t="str">
+        <f>IF(D18="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-javaplugin'!B2),"XXX",C18))</f>
+        <v>CobiGen Java Plug-in  (nachfolgend auch „cobigen-javaplugin“ genannt)</v>
+      </c>
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="21"/>
@@ -1352,15 +1738,18 @@
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
-      <c r="C19" s="21" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="C19" s="21" t="str">
+        <f>t_av_property[[#Headers],[cobigen-propertyplugin]]</f>
+        <v>cobigen-propertyplugin</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="21" t="str">
+        <f>IF(D19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-propertyplugin'!B2),"XXX",C19))</f>
+        <v>CobiGen Property Plug-in  (nachfolgend auch „cobigen-propertyplugin“ genannt)</v>
+      </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
       <c r="I19" s="21"/>
@@ -1543,7 +1932,7 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15">
       <formula1>av_core</formula1>
     </dataValidation>
@@ -1557,7 +1946,10 @@
       <formula1>av_maven</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D18">
-      <formula1>#REF!</formula1>
+      <formula1>av_java</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D19">
+      <formula1>av_property</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,16 +1962,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:R31"/>
+  <dimension ref="B2:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
@@ -1594,7 +1986,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="16"/>
@@ -1605,31 +1997,29 @@
     </row>
     <row r="3" spans="2:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v4.0.0</v>
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D19</f>
+        <v>v4.1.0</v>
+      </c>
       <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="J7" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="J7" s="15"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
@@ -1643,15 +2033,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="15"/>
-      <c r="K8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E9" s="2" t="s">
@@ -1664,10 +2046,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="28"/>
-      <c r="K9" s="29" t="str">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K9:$K$9)),1,1)</f>
-        <v>SLF4J</v>
-      </c>
+      <c r="K9" s="29"/>
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
@@ -1682,120 +2061,106 @@
         <v>10</v>
       </c>
       <c r="J10" s="15"/>
-      <c r="K10" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K10)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E12" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="15"/>
-      <c r="K11" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K11)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="J12" s="15"/>
-      <c r="K12" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K12)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K12" s="29"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J13" s="15"/>
-      <c r="K13" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K13)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J14" s="15"/>
-      <c r="K14" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K14)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J15" s="15"/>
-      <c r="K15" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K15)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K15" s="29"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J16" s="15"/>
-      <c r="K16" s="29" t="e">
-        <f>INDEX(t_dep_core_400[],SMALL(ROW(t_dep_core_400[])-MIN(ROW(t_dep_core_400[]))+1,ROWS(K$9:$K16)),1,1)</f>
-        <v>#NUM!</v>
-      </c>
+      <c r="K16" s="29"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+    <row r="17" spans="4:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="K17" s="3"/>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
@@ -1806,10 +2171,7 @@
     <row r="18" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
+      <c r="K18" s="3"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
@@ -1894,13 +2256,13 @@
     </row>
     <row r="23" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="J23" s="12"/>
       <c r="K23" s="12"/>
@@ -1914,13 +2276,13 @@
     </row>
     <row r="24" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E24" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -1934,10 +2296,10 @@
     </row>
     <row r="25" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -1954,10 +2316,10 @@
     </row>
     <row r="26" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E26" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>10</v>
@@ -1974,10 +2336,10 @@
     </row>
     <row r="27" spans="4:18" x14ac:dyDescent="0.25">
       <c r="E27" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>10</v>
@@ -1992,12 +2354,12 @@
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18" ht="30" x14ac:dyDescent="0.25">
       <c r="E28" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>10</v>
@@ -2012,16 +2374,7 @@
       <c r="Q28" s="12"/>
       <c r="R28" s="12"/>
     </row>
-    <row r="29" spans="4:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>10</v>
-      </c>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
@@ -2043,25 +2396,13 @@
       <c r="Q30" s="12"/>
       <c r="R30" s="12"/>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="3">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
-    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2070,14 +2411,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
@@ -2090,7 +2431,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="16"/>
@@ -2101,18 +2442,14 @@
     </row>
     <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v2.1.0</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -2121,8 +2458,12 @@
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D16</f>
+        <v>v3.0.0</v>
+      </c>
       <c r="D7" s="15" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -2150,206 +2491,177 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E13" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen Plug-ins."</f>
+        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core und allen Plug-ins.</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E14" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and the OSS components of all listed plug-ins."</f>
+        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of cobigen-core and the OSS components of all listed plug-ins.</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E15" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G22" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="s">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G24" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G25" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
+    <row r="26" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G26" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E26" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>10</v>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core.</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
       </c>
     </row>
   </sheetData>
@@ -2367,14 +2679,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
@@ -2387,7 +2699,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="16"/>
@@ -2398,18 +2710,14 @@
     </row>
     <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
-        <v>30</v>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v2.1.0</v>
       </c>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
@@ -2418,8 +2726,12 @@
       <c r="P6" s="17"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D19</f>
+        <v>v3.0.0</v>
+      </c>
       <c r="D7" s="15" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -2447,32 +2759,32 @@
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>10</v>
@@ -2480,22 +2792,21 @@
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K13" s="3"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
@@ -2503,29 +2814,22 @@
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen Plug-ins."</f>
+        <v>DE:Das CobiGen Maven Plug-in (cobigen-maven) wird gemeinsam mit cobigen-core und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core und allen Plug-ins.</v>
+      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="2"/>
+      <c r="E17" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and the OSS components of all listed plug-ins."</f>
+        <v>EN:The CobiGen Maven Plug-in (cobigen-maven) will be shipped with an integrated version of cobigen-core and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of cobigen-core and the OSS components of all listed plug-ins.</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
@@ -2534,7 +2838,7 @@
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="15" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2563,43 +2867,43 @@
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E22" s="6" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E23" s="4" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E24" s="6" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E25" s="4" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>10</v>
@@ -2607,7 +2911,7 @@
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="E26" s="6" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>21</v>
@@ -2616,38 +2920,386 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="5" t="s">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Maven Plug-in (cobigen-maven) wird gemeinsam mit cobigen-core. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core.</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_maven[[#Headers],[cobigen-maven]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Maven Plug-in (cobigen-maven) will be shipped with an integrated version of cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="33"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.5.0</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="str">
+        <f>D16</f>
+        <v>v1.6.0</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G28" s="7" t="s">
+    <row r="11" spans="2:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E29" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F29" s="8" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="E13" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; B4 &amp; ")  wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Java Plug-in (cobigen-javaplugin)  wird gemeinsam mit cobigen-core ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von cobigen-core.</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="E14" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; B4 &amp; ") will only be shipped together with " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Java Plug-in (cobigen-javaplugin) will only be shipped together with cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="D16" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="G20" s="5" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.1.1</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="str">
+        <f>D14</f>
+        <v>v1.2.0</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="E11" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; B4 &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Property Plug-in (cobigen-propertyplugin) wird gemeinsam mit cobigen-core ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von cobigen-core.</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="E12" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; B4 &amp; ") will only be shipped together with " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Property Plug-in (cobigen-propertyplugin) will only be shipped together with cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="D14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="E15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dynamic generation and minor fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/cobigen-licenses-include.xlsx
+++ b/src/main/resources/cobigen-licenses-include.xlsx
@@ -9,15 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" tabRatio="896"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" tabRatio="896" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="SELECTION" sheetId="1" r:id="rId1"/>
-    <sheet name="cobigen-core" sheetId="5" r:id="rId2"/>
-    <sheet name="cobigen-eclipse" sheetId="6" r:id="rId3"/>
+    <sheet name="cobigen-eclipse" sheetId="6" r:id="rId2"/>
+    <sheet name="cobigen-core" sheetId="5" r:id="rId3"/>
     <sheet name="cobigen-maven" sheetId="7" r:id="rId4"/>
     <sheet name="cobigen-javaplugin" sheetId="9" r:id="rId5"/>
     <sheet name="cobigen-propertyplugin" sheetId="10" r:id="rId6"/>
+    <sheet name="cobigen-xmlplugin" sheetId="11" r:id="rId7"/>
+    <sheet name="cobigen-textmerger" sheetId="13" r:id="rId8"/>
+    <sheet name="cobigen-jsonplugin" sheetId="14" r:id="rId9"/>
+    <sheet name="cobigen-htmlplugin" sheetId="15" r:id="rId10"/>
+    <sheet name="cobigen-tsplugin" sheetId="16" r:id="rId11"/>
+    <sheet name="cobigen-openapiplugin" sheetId="17" r:id="rId12"/>
+    <sheet name="cobigen-tempeng-freemarker" sheetId="18" r:id="rId13"/>
+    <sheet name="cobigen-tempeng-velocity" sheetId="19" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="av_core">t_av_core[cobigen-core]</definedName>
@@ -26,6 +34,8 @@
     <definedName name="av_maven">t_av_maven[cobigen-maven]</definedName>
     <definedName name="av_property">t_av_property[cobigen-propertyplugin]</definedName>
     <definedName name="languages">t_desc[Language]</definedName>
+    <definedName name="t_av_tempengvelocity">t_av_property353739[cobigen-tempeng-velocity]</definedName>
+    <definedName name="t_av_tsplugin">t_av_property23262932[cobigen-tsplugin]</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -37,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="109">
   <si>
     <t>cobigen-core</t>
   </si>
@@ -241,6 +251,129 @@
   </si>
   <si>
     <t>DE:Noch ein Kommentar.</t>
+  </si>
+  <si>
+    <t>CobiGen XML Plug-in</t>
+  </si>
+  <si>
+    <t>cobigen-xmlplugin</t>
+  </si>
+  <si>
+    <t>v3.1.0</t>
+  </si>
+  <si>
+    <t>LeXeMe</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>CobiGen Text Merger</t>
+  </si>
+  <si>
+    <t>cobigen-textmerger</t>
+  </si>
+  <si>
+    <t>v1.1.0</t>
+  </si>
+  <si>
+    <t>CobiGen Json Plugin</t>
+  </si>
+  <si>
+    <t>JSON In Java</t>
+  </si>
+  <si>
+    <t>20160810</t>
+  </si>
+  <si>
+    <t>Google-gson</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>CobiGen HTML Plugin</t>
+  </si>
+  <si>
+    <t>cobigen-htmlplugin</t>
+  </si>
+  <si>
+    <t>v1.0.0</t>
+  </si>
+  <si>
+    <t>JSOUP</t>
+  </si>
+  <si>
+    <t>1.10.2</t>
+  </si>
+  <si>
+    <t>CobiGen TS Plugin</t>
+  </si>
+  <si>
+    <t>cobigen-tsplugin</t>
+  </si>
+  <si>
+    <t>Rhino</t>
+  </si>
+  <si>
+    <t>1.7R4</t>
+  </si>
+  <si>
+    <t>Mozilla Public License 2.0</t>
+  </si>
+  <si>
+    <t>Ts-merger</t>
+  </si>
+  <si>
+    <t>Js-Beautify</t>
+  </si>
+  <si>
+    <t>1.6.3</t>
+  </si>
+  <si>
+    <t>DE:Das Plug-in cobigen-tsplugin wird gemeinsam mit cobigen-core ausgeliefert. Eine Auslieferung enthält somit auch alle OSS-Komponenten von cobigen-core.</t>
+  </si>
+  <si>
+    <t>2.0.0</t>
+  </si>
+  <si>
+    <t>1.6.14</t>
+  </si>
+  <si>
+    <t>CobiGen Tempeng Freemarker</t>
+  </si>
+  <si>
+    <t>cobigen-tempeng-freemarker</t>
+  </si>
+  <si>
+    <t>FreeMarker</t>
+  </si>
+  <si>
+    <t>2.3.23</t>
+  </si>
+  <si>
+    <t>BSD-style License</t>
+  </si>
+  <si>
+    <t>CobiGen Tempeng Velocity</t>
+  </si>
+  <si>
+    <t>cobigen-tempeng-velocity</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>cobigen-jsonplugin</t>
+  </si>
+  <si>
+    <t>cobigen-openapiplugin</t>
+  </si>
+  <si>
+    <t>CobiGen Open Api Plug-in</t>
   </si>
 </sst>
 </file>
@@ -371,7 +504,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -442,13 +575,67 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
   </cellStyles>
-  <dxfs count="59">
+  <dxfs count="129">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -562,7 +749,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -674,10 +861,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -784,10 +973,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -894,10 +1085,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1004,6 +1197,560 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1051,20 +1798,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="t_desc" displayName="t_desc" ref="F2:G4" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="t_desc" displayName="t_desc" ref="F2:G4" totalsRowShown="0" headerRowDxfId="128" dataDxfId="127">
   <tableColumns count="2">
-    <tableColumn id="1" name="Language" dataDxfId="56"/>
-    <tableColumn id="2" name="Description" dataDxfId="55"/>
+    <tableColumn id="1" name="Language" dataDxfId="126"/>
+    <tableColumn id="2" name="Description" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="t_av_maven" displayName="t_av_maven" ref="B4:B7" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="t_av_maven" displayName="t_av_maven" ref="B4:B7" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93">
   <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-maven" dataDxfId="22"/>
+    <tableColumn id="1" name="cobigen-maven" dataDxfId="92"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1074,31 +1821,31 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="t_dep_java_150" displayName="t_dep_java_150" ref="E8:G11" totalsRowShown="0">
   <autoFilter ref="E8:G11"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="21"/>
-    <tableColumn id="2" name="Version" dataDxfId="20"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="19"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="91"/>
+    <tableColumn id="2" name="Version" dataDxfId="90"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="t_dep_core_41013163" displayName="t_dep_core_41013163" ref="E17:G21" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="t_dep_core_41013163" displayName="t_dep_core_41013163" ref="E17:G21" totalsRowShown="0" headerRowBorderDxfId="88" tableBorderDxfId="87">
   <autoFilter ref="E17:G21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="16"/>
-    <tableColumn id="2" name="Version" dataDxfId="15"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="14"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="86"/>
+    <tableColumn id="2" name="Version" dataDxfId="85"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="84"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="t_av_java" displayName="t_av_java" ref="B4:B7" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="t_av_java" displayName="t_av_java" ref="B4:B7" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-javaplugin" dataDxfId="11"/>
+    <tableColumn id="1" name="cobigen-javaplugin" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1108,17 +1855,281 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="t_dep_java_1505" displayName="t_dep_java_1505" ref="E8:G9" totalsRowShown="0">
   <autoFilter ref="E8:G9"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="10"/>
-    <tableColumn id="2" name="Version" dataDxfId="9"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="8"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="80"/>
+    <tableColumn id="2" name="Version" dataDxfId="79"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="t_dep_core_410131636" displayName="t_dep_core_410131636" ref="E15:G16" totalsRowShown="0" headerRowBorderDxfId="7" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="t_dep_core_410131636" displayName="t_dep_core_410131636" ref="E15:G16" totalsRowShown="0" headerRowBorderDxfId="77" tableBorderDxfId="76">
   <autoFilter ref="E15:G16"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="75"/>
+    <tableColumn id="2" name="Version" dataDxfId="74"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="73"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="t_av_property" displayName="t_av_property" ref="B4:B7" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-propertyplugin" dataDxfId="70">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="t_dep_java_150518" displayName="t_dep_java_150518" ref="E8:G10" totalsRowShown="0">
+  <autoFilter ref="E8:G10"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="69"/>
+    <tableColumn id="2" name="Version" dataDxfId="68"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="67"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="t_dep_core_41013163619" displayName="t_dep_core_41013163619" ref="E16:G18" totalsRowShown="0" headerRowBorderDxfId="66" tableBorderDxfId="65">
+  <autoFilter ref="E16:G18"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="64"/>
+    <tableColumn id="2" name="Version" dataDxfId="63"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="62"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="t_av_xmlTable" displayName="t_av_xmlTable" ref="B4:B7" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-xmlplugin" dataDxfId="59">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="t_dep_core_40012" displayName="t_dep_core_40012" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="124"/>
+    <tableColumn id="2" name="Version" dataDxfId="123"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="122"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="t_dep_java_150521" displayName="t_dep_java_150521" ref="E8:G9" totalsRowShown="0">
+  <autoFilter ref="E8:G9"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="58"/>
+    <tableColumn id="2" name="Version" dataDxfId="57"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="56"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="t_dep_core_41013163622" displayName="t_dep_core_41013163622" ref="E13:G14" totalsRowShown="0" headerRowBorderDxfId="55" tableBorderDxfId="54">
+  <autoFilter ref="E13:G14"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="53"/>
+    <tableColumn id="2" name="Version" dataDxfId="52"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="51"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="t_av_textmerger" displayName="t_av_textmerger" ref="B4:B7" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-textmerger" dataDxfId="48">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="t_dep_java_15052124" displayName="t_dep_java_15052124" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="47"/>
+    <tableColumn id="2" name="Version" dataDxfId="46"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="t_dep_core_4101316362225" displayName="t_dep_core_4101316362225" ref="E16:G19" totalsRowShown="0" headerRowBorderDxfId="44" tableBorderDxfId="43">
+  <autoFilter ref="E16:G19"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="42"/>
+    <tableColumn id="2" name="Version" dataDxfId="41"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="40"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="t_av_property2326" displayName="t_av_property2326" ref="B4:B7" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-jsonplugin" dataDxfId="37">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="t_dep_java_1505212427" displayName="t_dep_java_1505212427" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="36"/>
+    <tableColumn id="2" name="Version" dataDxfId="35"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="34"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="t_dep_core_410131636222528" displayName="t_dep_core_410131636222528" ref="E16:G19" totalsRowShown="0" headerRowBorderDxfId="33" tableBorderDxfId="32">
+  <autoFilter ref="E16:G19"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="31"/>
+    <tableColumn id="2" name="Version" dataDxfId="30"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="29"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="t_av_property232629" displayName="t_av_property232629" ref="B4:B7" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-htmlplugin" dataDxfId="26">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="t_dep_java_150521242730" displayName="t_dep_java_150521242730" ref="E8:G12" totalsRowShown="0">
+  <autoFilter ref="E8:G12"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="25"/>
+    <tableColumn id="2" name="Version" dataDxfId="24"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="t_dep_core_41013" displayName="t_dep_core_41013" ref="E17:G26" totalsRowShown="0" headerRowBorderDxfId="121" tableBorderDxfId="120">
+  <autoFilter ref="E17:G26"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="119"/>
+    <tableColumn id="2" name="Version" dataDxfId="118"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="117"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="t_dep_core_41013163622252831" displayName="t_dep_core_41013163622252831" ref="E20:G23" totalsRowShown="0" headerRowBorderDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="E20:G23"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="20"/>
+    <tableColumn id="2" name="Version" dataDxfId="19"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="t_av_property23262932" displayName="t_av_property23262932" ref="B4:B7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-tsplugin" dataDxfId="15">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="34" name="t_av_property35" displayName="t_av_property35" ref="B4:B7" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-openapiplugin" dataDxfId="12">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="35" name="t_dep_java_15053336" displayName="t_dep_java_15053336" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="11"/>
+    <tableColumn id="2" name="Version" dataDxfId="10"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="36" name="t_av_property3537" displayName="t_av_property3537" ref="B4:B7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B4:B7"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="cobigen-tempeng-freemarker" dataDxfId="6">
+      <calculatedColumnFormula>D6</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="37" name="t_dep_java_1505333638" displayName="t_dep_java_1505333638" ref="E8:G11" totalsRowShown="0">
+  <autoFilter ref="E8:G11"/>
   <tableColumns count="3">
     <tableColumn id="1" name="OSS Komponente" dataDxfId="5"/>
     <tableColumn id="2" name="Version" dataDxfId="4"/>
@@ -1128,11 +2139,11 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="t_av_property" displayName="t_av_property" ref="B4:B7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="38" name="t_av_property353739" displayName="t_av_property353739" ref="B4:B7" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-propertyplugin" dataDxfId="0">
+    <tableColumn id="1" name="cobigen-tempeng-velocity" dataDxfId="0">
       <calculatedColumnFormula>D6</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1140,69 +2151,45 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="t_dep_core_400" displayName="t_dep_core_400" ref="E8:G17" totalsRowShown="0">
-  <autoFilter ref="E8:G17"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="54"/>
-    <tableColumn id="2" name="Version" dataDxfId="53"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="52"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="t_dep_core_410" displayName="t_dep_core_410" ref="E20:G28" totalsRowShown="0" headerRowBorderDxfId="51" tableBorderDxfId="50">
-  <autoFilter ref="E20:G28"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="49"/>
-    <tableColumn id="2" name="Version" dataDxfId="48"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="47"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="t_av_core" displayName="t_av_core" ref="B4:B7" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="t_av_eclipse" displayName="t_av_eclipse" ref="B4:B7" totalsRowShown="0" headerRowDxfId="116" dataDxfId="115">
   <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-core" dataDxfId="44"/>
+    <tableColumn id="1" name="cobigen-eclipse" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="t_dep_core_40012" displayName="t_dep_core_40012" ref="E8:G11" totalsRowShown="0">
-  <autoFilter ref="E8:G11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="t_dep_core_400" displayName="t_dep_core_400" ref="E8:G17" totalsRowShown="0">
+  <autoFilter ref="E8:G17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="43"/>
-    <tableColumn id="2" name="Version" dataDxfId="42"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="41"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="113"/>
+    <tableColumn id="2" name="Version" dataDxfId="112"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="t_dep_core_41013" displayName="t_dep_core_41013" ref="E17:G26" totalsRowShown="0" headerRowBorderDxfId="40" tableBorderDxfId="39">
-  <autoFilter ref="E17:G26"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="t_dep_core_410" displayName="t_dep_core_410" ref="E20:G28" totalsRowShown="0" headerRowBorderDxfId="110" tableBorderDxfId="109">
+  <autoFilter ref="E20:G28"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="38"/>
-    <tableColumn id="2" name="Version" dataDxfId="37"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="36"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="108"/>
+    <tableColumn id="2" name="Version" dataDxfId="107"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="106"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="t_av_eclipse" displayName="t_av_eclipse" ref="B4:B7" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="t_av_core" displayName="t_av_core" ref="B4:B7" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
   <autoFilter ref="B4:B7"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="cobigen-eclipse" dataDxfId="33"/>
+    <tableColumn id="1" name="cobigen-core" dataDxfId="103"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1212,21 +2199,21 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="t_dep_core_4001215" displayName="t_dep_core_4001215" ref="E8:G14" totalsRowShown="0">
   <autoFilter ref="E8:G14"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="32"/>
-    <tableColumn id="2" name="Version" dataDxfId="31"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="30"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="102"/>
+    <tableColumn id="2" name="Version" dataDxfId="101"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="t_dep_core_4101316" displayName="t_dep_core_4101316" ref="E20:G26" totalsRowShown="0" headerRowBorderDxfId="29" tableBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="t_dep_core_4101316" displayName="t_dep_core_4101316" ref="E20:G26" totalsRowShown="0" headerRowBorderDxfId="99" tableBorderDxfId="98">
   <autoFilter ref="E20:G26"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="OSS Komponente" dataDxfId="27"/>
-    <tableColumn id="2" name="Version" dataDxfId="26"/>
-    <tableColumn id="3" name="Lizenz" dataDxfId="25"/>
+    <tableColumn id="1" name="OSS Komponente" dataDxfId="97"/>
+    <tableColumn id="2" name="Version" dataDxfId="96"/>
+    <tableColumn id="3" name="Lizenz" dataDxfId="95"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1497,8 +2484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,7 +2606,7 @@
         <v>cobigen-eclipse</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E11" s="21"/>
       <c r="F11" s="21" t="str">
@@ -1723,8 +2710,9 @@
         <f>t_av_java[[#Headers],[cobigen-javaplugin]]</f>
         <v>cobigen-javaplugin</v>
       </c>
-      <c r="D18" s="24" t="s">
-        <v>31</v>
+      <c r="D18" s="24" t="str">
+        <f>IF(ISNUMBER(SEARCH("v2.1.0",D11)),"v1.5.0",IF(ISNUMBER(SEARCH("v3.0.0",D11)),"",""))</f>
+        <v>v1.5.0</v>
       </c>
       <c r="E18" s="21"/>
       <c r="F18" s="21" t="str">
@@ -1742,13 +2730,11 @@
         <f>t_av_property[[#Headers],[cobigen-propertyplugin]]</f>
         <v>cobigen-propertyplugin</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>66</v>
-      </c>
+      <c r="D19" s="24"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21" t="str">
         <f>IF(D19="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-propertyplugin'!B2),"XXX",C19))</f>
-        <v>CobiGen Property Plug-in  (nachfolgend auch „cobigen-propertyplugin“ genannt)</v>
+        <v/>
       </c>
       <c r="G19" s="21"/>
       <c r="H19" s="21"/>
@@ -1757,10 +2743,16 @@
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21"/>
       <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
+      <c r="C20" s="21" t="str">
+        <f>'cobigen-xmlplugin'!B4</f>
+        <v>cobigen-xmlplugin</v>
+      </c>
       <c r="D20" s="24"/>
       <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="21" t="str">
+        <f>IF(D20="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-xmlplugin'!B2),"XXX",C20))</f>
+        <v/>
+      </c>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
       <c r="I20" s="21"/>
@@ -1768,10 +2760,16 @@
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
       <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="C21" s="21" t="str">
+        <f>'cobigen-textmerger'!B4</f>
+        <v>cobigen-textmerger</v>
+      </c>
       <c r="D21" s="24"/>
       <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="21" t="str">
+        <f>IF(D21="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-textmerger'!B2),"XXX",C21))</f>
+        <v/>
+      </c>
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="21"/>
@@ -1779,10 +2777,16 @@
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
+      <c r="C22" s="21" t="str">
+        <f>'cobigen-jsonplugin'!B4</f>
+        <v>cobigen-jsonplugin</v>
+      </c>
       <c r="D22" s="24"/>
       <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="F22" s="21" t="str">
+        <f>IF(D22="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-jsonplugin'!B2),"XXX",C22))</f>
+        <v/>
+      </c>
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
@@ -1790,54 +2794,93 @@
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="24"/>
+      <c r="C23" s="21" t="str">
+        <f>'cobigen-htmlplugin'!B4</f>
+        <v>cobigen-htmlplugin</v>
+      </c>
+      <c r="D23" s="24" t="str">
+        <f>IF(ISNUMBER(SEARCH("v2.1.0",D11)),"v1.0.0",IF(ISNUMBER(SEARCH("v3.0.0",D11)),"",""))</f>
+        <v>v1.0.0</v>
+      </c>
       <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="21" t="str">
+        <f>IF(D23="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-htmlplugin'!B2),"XXX",C23))</f>
+        <v>CobiGen HTML Plugin  (nachfolgend auch „cobigen-htmlplugin“ genannt)</v>
+      </c>
       <c r="G23" s="21"/>
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="21" t="str">
+        <f>'cobigen-tsplugin'!B4</f>
+        <v>cobigen-tsplugin</v>
+      </c>
+      <c r="D24" s="24" t="str">
+        <f>IF(ISNUMBER(SEARCH("v2.1.0",D11)),"v1.0.0",IF(ISNUMBER(SEARCH("v3.0.0",D11)),"",""))</f>
+        <v>v1.0.0</v>
+      </c>
       <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="F24" s="21" t="str">
+        <f>IF(D24="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-tsplugin'!B2),"XXX",C24))</f>
+        <v>CobiGen TS Plugin  (nachfolgend auch „cobigen-tsplugin“ genannt)</v>
+      </c>
       <c r="G24" s="21"/>
       <c r="H24" s="21"/>
       <c r="I24" s="21"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="C25" s="21" t="str">
+        <f>'cobigen-openapiplugin'!B4</f>
+        <v>cobigen-openapiplugin</v>
+      </c>
+      <c r="D25" s="24"/>
       <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="F25" s="21" t="str">
+        <f>IF(D25="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-openapiplugin'!B2),"XXX",C25))</f>
+        <v/>
+      </c>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="21"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
       <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="21" t="str">
+        <f>'cobigen-tempeng-freemarker'!B4</f>
+        <v>cobigen-tempeng-freemarker</v>
+      </c>
+      <c r="D26" s="24" t="str">
+        <f>IF(ISNUMBER(SEARCH("v2.1.0",D11)),"v1.0.0",IF(ISNUMBER(SEARCH("v3.0.0",D11)),"",""))</f>
+        <v>v1.0.0</v>
+      </c>
       <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="F26" s="21" t="str">
+        <f>IF(D26="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-tempeng-freemarker'!B2),"XXX",C26))</f>
+        <v>CobiGen Tempeng Freemarker  (nachfolgend auch „cobigen-tempeng-freemarker“ genannt)</v>
+      </c>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="21"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
+      <c r="C27" s="21" t="str">
+        <f>'cobigen-tempeng-velocity'!B4</f>
+        <v>cobigen-tempeng-velocity</v>
+      </c>
+      <c r="D27" s="24"/>
       <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="F27" s="21" t="str">
+        <f>IF(D27="","",SUBSTITUTE(SUBSTITUTE(VLOOKUP(C2,t_desc[],2,FALSE),"NAME",'cobigen-tempeng-velocity'!B2),"XXX",C27))</f>
+        <v/>
+      </c>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="21"/>
@@ -1953,8 +2996,1090 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-xmlplugin'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D20</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-textmerger'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D21:D22</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-htmlplugin'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D23</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-tsplugin'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D24</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-openapiplugin'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D25</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-tempeng-freemarker'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D26</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'cobigen-tempeng-velocity'!$B$5:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>D27</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.0.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34" t="str">
+        <f>D13</f>
+        <v>v1.1.0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.0.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34" t="str">
+        <f>D17</f>
+        <v>v1.1.0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="2"/>
+      <c r="E15" s="31" t="str">
+        <f>"EN:The Plug-in cobigen-tsplugin will only be shipped together with " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The Plug-in cobigen-tsplugin will only be shipped together with cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D18" s="15"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D19" s="15"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.0.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.0.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.0.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
@@ -1962,10 +4087,278 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:P29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v2.1.0</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="str">
+        <f>D16</f>
+        <v>v3.0.0</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E13" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen Plug-ins."</f>
+        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core und allen Plug-ins.</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E14" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and the OSS components of all listed plug-ins."</f>
+        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of cobigen-core and the OSS components of all listed plug-ins.</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="E15" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core.</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,279 +4800,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:P29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="59.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:16" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="2:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="str">
-        <f>D7</f>
-        <v>v2.1.0</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="str">
-        <f>D16</f>
-        <v>v3.0.0</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E13" s="31" t="str">
-        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " und allen Plug-ins."</f>
-        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core und allen unter 1.2.1 gelisteten Plug-ins ausgeliefert. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core und allen Plug-ins.</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E14" s="31" t="str">
-        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " and the OSS components of all listed plug-ins."</f>
-        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core and with all plug-ins integrated listed under section 1.2.1. The delivered artifacts thus also contain the OSS components of cobigen-core and the OSS components of all listed plug-ins.</v>
-      </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="E15" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="5:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="E26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="12" t="str">
-        <f>"DE:Das " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
-        <v>DE:Das CobiGen Eclipse Plug-in (cobigen-eclipse) wird gemeinsam mit cobigen-core. Die Auslieferung enthält somit auch alle in diesem Kapitel gelisteten OSS-Komponenten von cobigen-core.</v>
-      </c>
-    </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="31" t="str">
-        <f>"EN:The " &amp; B2 &amp; " (" &amp; t_av_eclipse[[#Headers],[cobigen-eclipse]] &amp; ") will be shipped with an integrated version of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
-        <v>EN:The CobiGen Eclipse Plug-in (cobigen-eclipse) will be shipped with an integrated version of cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="3">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
-  </tableParts>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2947,18 +5072,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
@@ -3155,17 +5280,17 @@
   <dimension ref="B2:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="14" style="2" customWidth="1"/>
     <col min="4" max="4" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
@@ -3310,4 +5435,790 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v3.0.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="str">
+        <f>D15</f>
+        <v>v3.1.0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="31" t="str">
+        <f>"DE:Das " &amp; B2 &amp; " (" &amp; B4 &amp; ") wird gemeinsam mit " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; " ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>DE:Das CobiGen XML Plug-in (cobigen-xmlplugin) wird gemeinsam mit cobigen-core ausgeliefert. Die Auslieferung enthält somit auch alle OSS-Komponenten von cobigen-core.</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="31" t="str">
+        <f>"EN:The " &amp; B2 &amp; " (" &amp; B4 &amp; ") will only be shipped together with " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; ". The delivered artifacts thus also contain the OSS components of " &amp; t_av_core[[#Headers],[cobigen-core]] &amp; "."</f>
+        <v>EN:The CobiGen XML Plug-in (cobigen-xmlplugin) will only be shipped together with cobigen-core. The delivered artifacts thus also contain the OSS components of cobigen-core.</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="C14" s="2"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
+      <c r="C18" s="2"/>
+      <c r="E18" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="35"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.1.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34" t="str">
+        <f>D12</f>
+        <v>v1.2.0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="2"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="2"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="str">
+        <f>D7</f>
+        <v>v1.1.0</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="34" t="str">
+        <f>D13</f>
+        <v>v1.2.0</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4">
+        <v>20160810</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>